<commit_message>
merge con lista feature principale
</commit_message>
<xml_diff>
--- a/data/FeatureListElsa.xlsx
+++ b/data/FeatureListElsa.xlsx
@@ -1407,6 +1407,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G136" totalsRowShown="0">
+  <autoFilter ref="A1:G136"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Module"/>
+    <tableColumn id="2" name="Functionality"/>
+    <tableColumn id="3" name="Tag"/>
+    <tableColumn id="4" name="Discontinued"/>
+    <tableColumn id="5" name="Fragment"/>
+    <tableColumn id="6" name="AllowISO"/>
+    <tableColumn id="7" name="DenyISO"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1673,13 +1689,14 @@
   <dimension ref="A1:G136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="36.5703125" customWidth="1"/>
     <col min="6" max="8" width="75.28515625" customWidth="1"/>
   </cols>
@@ -3481,5 +3498,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>